<commit_message>
Add some of FX
</commit_message>
<xml_diff>
--- a/Assets/Design/workNedd0620.xlsx
+++ b/Assets/Design/workNedd0620.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26240" windowHeight="13400" tabRatio="812"/>
+    <workbookView windowWidth="26240" windowHeight="13400" tabRatio="812" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="122">
   <si>
     <t>solved</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>加入下一轮会有什么卡牌功能？</t>
+  </si>
+  <si>
+    <t>浅灰色的朱鹮</t>
   </si>
   <si>
     <t>若将物件放入死路，ibisA会永远卡死在外面</t>
@@ -1428,7 +1431,7 @@
   <sheetPr/>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" topLeftCell="A2" workbookViewId="0">
+    <sheetView zoomScale="133" zoomScaleNormal="133" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1868,8 +1871,8 @@
   <sheetPr/>
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" outlineLevelCol="5"/>
@@ -2128,6 +2131,11 @@
     <row r="17" s="1" customFormat="1" spans="6:6">
       <c r="F17" s="1" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="6:6">
+      <c r="F18" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2183,10 +2191,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2197,7 +2205,7 @@
         <v>0.5</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2208,12 +2216,12 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2248,112 +2256,112 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="1" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" spans="1:1">
       <c r="A21" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2378,61 +2386,61 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2454,15 +2462,15 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B2">
         <v>6.8</v>
@@ -2473,7 +2481,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B3">
         <v>12.75</v>
@@ -2484,7 +2492,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B4">
         <v>5.75</v>
@@ -2495,7 +2503,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B6">
         <f>SUM(B2:B4)</f>
@@ -2528,7 +2536,7 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>